<commit_message>
Populate forms with previous data.
</commit_message>
<xml_diff>
--- a/odk_app/config/tables/prev_data/forms/prev_data/prev_data.xlsx
+++ b/odk_app/config/tables/prev_data/forms/prev_data/prev_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\dev\classes\capstone\app-designer-2.1.6\app\config\tables\prev_data\forms\prev_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E14BB5E-E750-438E-BF50-931E2478D016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2479709-152B-465D-BDB9-B5B7636B5F1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24330" yWindow="7890" windowWidth="21600" windowHeight="11520" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24330" yWindow="7890" windowWidth="21600" windowHeight="11520" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="241">
   <si>
     <t>setting_name</t>
   </si>
@@ -466,289 +466,292 @@
     <t>lean_angle</t>
   </si>
   <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>tree_status</t>
+  </si>
+  <si>
+    <t>1 - Alive</t>
+  </si>
+  <si>
+    <t>2 - Ingrowth</t>
+  </si>
+  <si>
+    <t>3 - Fused at DBH</t>
+  </si>
+  <si>
+    <t>6 - Dead</t>
+  </si>
+  <si>
+    <t>9 - Not found</t>
+  </si>
+  <si>
+    <t>canopy_class</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>S - Suppressed</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>I - Intermediate</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C - Co-dominant</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>D - Dominant</t>
+  </si>
+  <si>
+    <t>species_list</t>
+  </si>
+  <si>
+    <t>ABAM</t>
+  </si>
+  <si>
+    <t>ABAM - Abies amabilis (Pacific silver fir)</t>
+  </si>
+  <si>
+    <t>ABCO</t>
+  </si>
+  <si>
+    <t>ABCO - Abies concolor (white fir)</t>
+  </si>
+  <si>
+    <t>ABGR</t>
+  </si>
+  <si>
+    <t>ABGR - Abies grandis (grand fir)</t>
+  </si>
+  <si>
+    <t>ABLA</t>
+  </si>
+  <si>
+    <t>ABLA - Abies lasiocarpa (subalpine fir)</t>
+  </si>
+  <si>
+    <t>ABMA</t>
+  </si>
+  <si>
+    <t>ABMA - Abies magnifica (Shasta red fir)</t>
+  </si>
+  <si>
+    <t>ABPR</t>
+  </si>
+  <si>
+    <t>ABPR - Abies procera (noble fir)</t>
+  </si>
+  <si>
+    <t>ACGL</t>
+  </si>
+  <si>
+    <t>ACGL - Acer glabrum (Rocky Mtn maple)</t>
+  </si>
+  <si>
+    <t>ACMA3</t>
+  </si>
+  <si>
+    <t>ACMA3 - Acer macrophyllum (bigleaf maple)</t>
+  </si>
+  <si>
+    <t>ALRU2</t>
+  </si>
+  <si>
+    <t>ALRU2 - Alnus rubra (red alder)</t>
+  </si>
+  <si>
+    <t>ALVIS</t>
+  </si>
+  <si>
+    <t>ALVIS - Alnus viridis ssp sinuata (Sitka alder)</t>
+  </si>
+  <si>
+    <t>ARME</t>
+  </si>
+  <si>
+    <t>ARME - Arbutus menziesii (Pacific madrone)</t>
+  </si>
+  <si>
+    <t>CHCH7</t>
+  </si>
+  <si>
+    <t>CHCH7 - Chrysolepis chrysophylla (golden chinquapin)</t>
+  </si>
+  <si>
+    <t>CADE27</t>
+  </si>
+  <si>
+    <t>CADE27 - Calocedrus decurrens (incense cedar)</t>
+  </si>
+  <si>
+    <t>CANO9</t>
+  </si>
+  <si>
+    <t>CANO9 - Callitropsis nootkatensis (Alaska yellow cedar)</t>
+  </si>
+  <si>
+    <t>CONU4</t>
+  </si>
+  <si>
+    <t>CONU4 - Cornus nuttalli (Pacific dogwood)</t>
+  </si>
+  <si>
+    <t>FRPU7</t>
+  </si>
+  <si>
+    <t>FRPU7 - Frangula purshiana (Cascara buckthorn)</t>
+  </si>
+  <si>
+    <t>PICO</t>
+  </si>
+  <si>
+    <t>PICO - Pinus contorta (Lodgepole pine)</t>
+  </si>
+  <si>
+    <t>PIEN</t>
+  </si>
+  <si>
+    <t>PIEN - Picea engelmanii (Engelmnn spruce)</t>
+  </si>
+  <si>
+    <t>PILA</t>
+  </si>
+  <si>
+    <t>PILA - Pinus lambertiana (sugar pine)</t>
+  </si>
+  <si>
+    <t>PIMO3</t>
+  </si>
+  <si>
+    <t>PIMO3 - Pinus monticola (w. white pine)</t>
+  </si>
+  <si>
+    <t>PIPO</t>
+  </si>
+  <si>
+    <t>PIPO - Pinus ponderosa (ponderosa pine)</t>
+  </si>
+  <si>
+    <t>PISI</t>
+  </si>
+  <si>
+    <t>PISI - Picea sitchensis (Sitka spruce)</t>
+  </si>
+  <si>
+    <t>POBAT</t>
+  </si>
+  <si>
+    <t>POBAT - Populus balsamifer v. trich. (black cottonwood)</t>
+  </si>
+  <si>
+    <t>PREM</t>
+  </si>
+  <si>
+    <t>PREM - Prunus emarginata (bitter cherry)</t>
+  </si>
+  <si>
+    <t>PRUNU</t>
+  </si>
+  <si>
+    <t>PRUNU - Prunus spp. (cherry)</t>
+  </si>
+  <si>
+    <t>PSME</t>
+  </si>
+  <si>
+    <t>PSME - Pseudotsuga menziesii (Douglas-fir)</t>
+  </si>
+  <si>
+    <t>QUGA4</t>
+  </si>
+  <si>
+    <t>QUGA4 - Quercus garryana (Oregon white oak)</t>
+  </si>
+  <si>
+    <t>QUKE</t>
+  </si>
+  <si>
+    <t>QUKE - Quercus kelloggii (California black oak)</t>
+  </si>
+  <si>
+    <t>TABR2</t>
+  </si>
+  <si>
+    <t>TABR2 - Taxus brevifolia (Pacific yew)</t>
+  </si>
+  <si>
+    <t>THPL</t>
+  </si>
+  <si>
+    <t>THPL - Thuja plicata (western redcedar)</t>
+  </si>
+  <si>
+    <t>TSHE</t>
+  </si>
+  <si>
+    <t>TSHE - Tsuga heterophylla (western hemlock)</t>
+  </si>
+  <si>
+    <t>TSME</t>
+  </si>
+  <si>
+    <t>TSME - Tsuga mertensiana (mountain hemlock)</t>
+  </si>
+  <si>
+    <t>Stand</t>
+  </si>
+  <si>
+    <t>Plot</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>DBH</t>
+  </si>
+  <si>
+    <t>Main stem</t>
+  </si>
+  <si>
+    <t>Lean angle</t>
+  </si>
+  <si>
+    <t>Previous comments</t>
+  </si>
+  <si>
     <t>comments</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>yes_no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>tree_status</t>
-  </si>
-  <si>
-    <t>1 - Alive</t>
-  </si>
-  <si>
-    <t>2 - Ingrowth</t>
-  </si>
-  <si>
-    <t>3 - Fused at DBH</t>
-  </si>
-  <si>
-    <t>6 - Dead</t>
-  </si>
-  <si>
-    <t>9 - Not found</t>
-  </si>
-  <si>
-    <t>canopy_class</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>S - Suppressed</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>I - Intermediate</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>C - Co-dominant</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>D - Dominant</t>
-  </si>
-  <si>
-    <t>species_list</t>
-  </si>
-  <si>
-    <t>ABAM</t>
-  </si>
-  <si>
-    <t>ABAM - Abies amabilis (Pacific silver fir)</t>
-  </si>
-  <si>
-    <t>ABCO</t>
-  </si>
-  <si>
-    <t>ABCO - Abies concolor (white fir)</t>
-  </si>
-  <si>
-    <t>ABGR</t>
-  </si>
-  <si>
-    <t>ABGR - Abies grandis (grand fir)</t>
-  </si>
-  <si>
-    <t>ABLA</t>
-  </si>
-  <si>
-    <t>ABLA - Abies lasiocarpa (subalpine fir)</t>
-  </si>
-  <si>
-    <t>ABMA</t>
-  </si>
-  <si>
-    <t>ABMA - Abies magnifica (Shasta red fir)</t>
-  </si>
-  <si>
-    <t>ABPR</t>
-  </si>
-  <si>
-    <t>ABPR - Abies procera (noble fir)</t>
-  </si>
-  <si>
-    <t>ACGL</t>
-  </si>
-  <si>
-    <t>ACGL - Acer glabrum (Rocky Mtn maple)</t>
-  </si>
-  <si>
-    <t>ACMA3</t>
-  </si>
-  <si>
-    <t>ACMA3 - Acer macrophyllum (bigleaf maple)</t>
-  </si>
-  <si>
-    <t>ALRU2</t>
-  </si>
-  <si>
-    <t>ALRU2 - Alnus rubra (red alder)</t>
-  </si>
-  <si>
-    <t>ALVIS</t>
-  </si>
-  <si>
-    <t>ALVIS - Alnus viridis ssp sinuata (Sitka alder)</t>
-  </si>
-  <si>
-    <t>ARME</t>
-  </si>
-  <si>
-    <t>ARME - Arbutus menziesii (Pacific madrone)</t>
-  </si>
-  <si>
-    <t>CHCH7</t>
-  </si>
-  <si>
-    <t>CHCH7 - Chrysolepis chrysophylla (golden chinquapin)</t>
-  </si>
-  <si>
-    <t>CADE27</t>
-  </si>
-  <si>
-    <t>CADE27 - Calocedrus decurrens (incense cedar)</t>
-  </si>
-  <si>
-    <t>CANO9</t>
-  </si>
-  <si>
-    <t>CANO9 - Callitropsis nootkatensis (Alaska yellow cedar)</t>
-  </si>
-  <si>
-    <t>CONU4</t>
-  </si>
-  <si>
-    <t>CONU4 - Cornus nuttalli (Pacific dogwood)</t>
-  </si>
-  <si>
-    <t>FRPU7</t>
-  </si>
-  <si>
-    <t>FRPU7 - Frangula purshiana (Cascara buckthorn)</t>
-  </si>
-  <si>
-    <t>PICO</t>
-  </si>
-  <si>
-    <t>PICO - Pinus contorta (Lodgepole pine)</t>
-  </si>
-  <si>
-    <t>PIEN</t>
-  </si>
-  <si>
-    <t>PIEN - Picea engelmanii (Engelmnn spruce)</t>
-  </si>
-  <si>
-    <t>PILA</t>
-  </si>
-  <si>
-    <t>PILA - Pinus lambertiana (sugar pine)</t>
-  </si>
-  <si>
-    <t>PIMO3</t>
-  </si>
-  <si>
-    <t>PIMO3 - Pinus monticola (w. white pine)</t>
-  </si>
-  <si>
-    <t>PIPO</t>
-  </si>
-  <si>
-    <t>PIPO - Pinus ponderosa (ponderosa pine)</t>
-  </si>
-  <si>
-    <t>PISI</t>
-  </si>
-  <si>
-    <t>PISI - Picea sitchensis (Sitka spruce)</t>
-  </si>
-  <si>
-    <t>POBAT</t>
-  </si>
-  <si>
-    <t>POBAT - Populus balsamifer v. trich. (black cottonwood)</t>
-  </si>
-  <si>
-    <t>PREM</t>
-  </si>
-  <si>
-    <t>PREM - Prunus emarginata (bitter cherry)</t>
-  </si>
-  <si>
-    <t>PRUNU</t>
-  </si>
-  <si>
-    <t>PRUNU - Prunus spp. (cherry)</t>
-  </si>
-  <si>
-    <t>PSME</t>
-  </si>
-  <si>
-    <t>PSME - Pseudotsuga menziesii (Douglas-fir)</t>
-  </si>
-  <si>
-    <t>QUGA4</t>
-  </si>
-  <si>
-    <t>QUGA4 - Quercus garryana (Oregon white oak)</t>
-  </si>
-  <si>
-    <t>QUKE</t>
-  </si>
-  <si>
-    <t>QUKE - Quercus kelloggii (California black oak)</t>
-  </si>
-  <si>
-    <t>TABR2</t>
-  </si>
-  <si>
-    <t>TABR2 - Taxus brevifolia (Pacific yew)</t>
-  </si>
-  <si>
-    <t>THPL</t>
-  </si>
-  <si>
-    <t>THPL - Thuja plicata (western redcedar)</t>
-  </si>
-  <si>
-    <t>TSHE</t>
-  </si>
-  <si>
-    <t>TSHE - Tsuga heterophylla (western hemlock)</t>
-  </si>
-  <si>
-    <t>TSME</t>
-  </si>
-  <si>
-    <t>TSME - Tsuga mertensiana (mountain hemlock)</t>
-  </si>
-  <si>
-    <t>Stand</t>
-  </si>
-  <si>
-    <t>Plot</t>
-  </si>
-  <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>DBH</t>
-  </si>
-  <si>
-    <t>Main stem</t>
-  </si>
-  <si>
-    <t>Lean angle</t>
   </si>
 </sst>
 </file>
@@ -1362,15 +1365,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5703125"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" customWidth="1"/>
     <col min="6" max="7" width="4.42578125" customWidth="1"/>
@@ -1408,7 +1411,7 @@
         <v>126</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1419,7 +1422,7 @@
         <v>127</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1430,7 +1433,7 @@
         <v>128</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1438,13 +1441,13 @@
         <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
         <v>138</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1452,13 +1455,13 @@
         <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
         <v>140</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I6" s="6"/>
     </row>
@@ -1470,7 +1473,7 @@
         <v>142</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1484,7 +1487,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1495,18 +1498,18 @@
         <v>144</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" t="s">
-        <v>145</v>
+        <v>240</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>145</v>
+        <v>239</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -1560,7 +1563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -1585,123 +1588,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
         <v>147</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>148</v>
-      </c>
-      <c r="C2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" t="s">
         <v>150</v>
-      </c>
-      <c r="C3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" t="s">
         <v>158</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>159</v>
-      </c>
-      <c r="C13" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" t="s">
         <v>161</v>
-      </c>
-      <c r="C14" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" t="s">
         <v>163</v>
-      </c>
-      <c r="C15" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C16" t="s">
         <v>165</v>
-      </c>
-      <c r="C16" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2367,354 +2370,354 @@
     </row>
     <row r="82" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>166</v>
+      </c>
+      <c r="B82" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="C82" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B83" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B84" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B85" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C85" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B86" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B87" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C87" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B88" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C88" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B89" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C89" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B90" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C90" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B91" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C91" s="8" t="s">
         <v>186</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B92" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C92" s="8" t="s">
         <v>188</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B93" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C93" s="8" t="s">
         <v>190</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B94" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C94" s="8" t="s">
         <v>192</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B95" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C95" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B96" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C96" s="8" t="s">
         <v>196</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B97" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C97" s="8" t="s">
         <v>198</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B98" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C98" s="8" t="s">
         <v>200</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B99" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C99" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B100" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C100" s="8" t="s">
         <v>204</v>
-      </c>
-      <c r="C100" s="8" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B101" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C101" s="8" t="s">
         <v>206</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B102" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C102" s="8" t="s">
         <v>208</v>
-      </c>
-      <c r="C102" s="8" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B103" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C103" s="8" t="s">
         <v>210</v>
-      </c>
-      <c r="C103" s="8" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B104" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C104" s="8" t="s">
         <v>212</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B105" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C105" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="C105" s="8" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B106" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C106" s="8" t="s">
         <v>216</v>
-      </c>
-      <c r="C106" s="8" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B107" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C107" s="8" t="s">
         <v>218</v>
-      </c>
-      <c r="C107" s="8" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B108" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C108" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B109" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C109" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="C109" s="8" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B110" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C110" s="8" t="s">
         <v>224</v>
-      </c>
-      <c r="C110" s="8" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B111" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C111" s="8" t="s">
         <v>226</v>
-      </c>
-      <c r="C111" s="8" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B112" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C112" s="8" t="s">
         <v>228</v>
-      </c>
-      <c r="C112" s="8" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B113" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C113" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2732,7 +2735,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2815,10 +2818,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>